<commit_message>
Most of the UI is now polished, removed unwanted files & fonts.
</commit_message>
<xml_diff>
--- a/Unity/DesignDoc/PromoStrip_probability.xlsx
+++ b/Unity/DesignDoc/PromoStrip_probability.xlsx
@@ -14,23 +14,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Top Strip</t>
   </si>
   <si>
-    <t>Watch Video Ads</t>
-  </si>
-  <si>
     <t xml:space="preserve">Character buy </t>
   </si>
   <si>
     <t>Preview Locked characters to play for a while</t>
   </si>
   <si>
-    <t>Middle Strip</t>
-  </si>
-  <si>
     <t>Mission Complete Claim</t>
   </si>
   <si>
@@ -49,33 +43,15 @@
     <t>Use Gatcha (if coins available)</t>
   </si>
   <si>
-    <t>Rate Us (disable if clicked)</t>
-  </si>
-  <si>
-    <t>Facebook Connect (disable if clicked)</t>
-  </si>
-  <si>
-    <t>Google + / Apple Connect (disable if clicked)</t>
-  </si>
-  <si>
-    <t>Blank no message</t>
-  </si>
-  <si>
     <t>Promo Type</t>
   </si>
   <si>
-    <t>Probability</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
     <t>Gift to user</t>
   </si>
   <si>
-    <t>50 coins</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -85,7 +61,46 @@
     <t>250 coins</t>
   </si>
   <si>
-    <t>500 coins</t>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Watch Video Ads Earn Coins</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>if completed then</t>
+  </si>
+  <si>
+    <t>1. Show maximum of 2 banner strips at a time.</t>
+  </si>
+  <si>
+    <t>2. If player does not complete part of either mission or the collectible in the current session then show only 1 banner.</t>
+  </si>
+  <si>
+    <t>3. The banner shown have the following priorities in decreasing order,</t>
+  </si>
+  <si>
+    <t>a. Mission Remaining/Complete (1st banner position)</t>
+  </si>
+  <si>
+    <t>b. Collectible Remaining/Complete (2nd banner position)</t>
+  </si>
+  <si>
+    <t>c. Free Gift (every 60 mins. Make it tweakable). When the 60 mins are up, this gets higher priority over collectible remaining/complete. (2nd banner position)</t>
+  </si>
+  <si>
+    <t>d. Earn Coins (2nd banner position)</t>
+  </si>
+  <si>
+    <t>e. Free gift in X time (After free gift is claimed, show this immediately once and then show this every 3 make it (tweakable) sessions) (2nd banner position)</t>
+  </si>
+  <si>
+    <t>f. Direct character purchase offer. (2nd banner position)</t>
+  </si>
+  <si>
+    <t>The rate us, facebook connect, apple/google play connect are three buttons in the bottom left corner of the screen. We do not need a banner for it.</t>
   </si>
 </sst>
 </file>
@@ -442,200 +457,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="45.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="16" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3">
         <v>1</v>
       </c>
-      <c r="C3" s="3">
-        <v>70</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3">
-        <v>5</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3">
-        <v>5</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3">
-        <v>30</v>
-      </c>
-      <c r="D8" s="3" t="s">
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="3">
-        <v>10</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="3">
-        <v>30</v>
-      </c>
-      <c r="D10" s="3" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="3">
-        <v>10</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="3">
-        <v>20</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="3">
-        <v>45</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="3">
-        <v>10</v>
-      </c>
-      <c r="D15" s="3" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="3">
-        <v>10</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="3">
-        <v>10</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>20</v>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>